<commit_message>
Updated BOM to include mechanical parts.
</commit_message>
<xml_diff>
--- a/EFI+Ignition/PCB Files/BOM_Power_Buggy_EFI_V3.1.xlsx
+++ b/EFI+Ignition/PCB Files/BOM_Power_Buggy_EFI_V3.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Documents\John Patterson Consulting LLC\eagle\Power_Buggy_EFI\V3.0 (All-In-Nano)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB99ACF-71C1-4940-9437-18B6E04D38D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53392CB3-0370-4657-979C-AC1176787E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="18000" windowHeight="9398" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="67">
   <si>
     <t>Description:</t>
   </si>
@@ -172,13 +172,67 @@
   </si>
   <si>
     <t>1N5919BG</t>
+  </si>
+  <si>
+    <t>ARDUINO NANO</t>
+  </si>
+  <si>
+    <t>Suggested Mechanical Parts:</t>
+  </si>
+  <si>
+    <t>Engine Control Module Parts:</t>
+  </si>
+  <si>
+    <t>Source:</t>
+  </si>
+  <si>
+    <t>Fuel Injector Barb Adapter</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/113711584424</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/itm/223283676528</t>
+  </si>
+  <si>
+    <t>440 cc/min Fuel Injectors</t>
+  </si>
+  <si>
+    <t>MAP Sensor</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B07Z37XG1J</t>
+  </si>
+  <si>
+    <t>Fuel Filter/Pressure Regulator</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B07W9H5TF9</t>
+  </si>
+  <si>
+    <t>Fuel Pump</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B07J39HNTC</t>
+  </si>
+  <si>
+    <t>Fuel Hose</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B00PLKV5H6</t>
+  </si>
+  <si>
+    <t>High-Energy Ignition Coil (Sold as pack of 8, but only need 1)</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B00EOXZLG2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,6 +242,15 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -215,10 +278,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,69 +563,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="48.73046875" customWidth="1"/>
-    <col min="2" max="2" width="32.33203125" customWidth="1"/>
+    <col min="1" max="1" width="75.86328125" customWidth="1"/>
+    <col min="2" max="2" width="44.9296875" customWidth="1"/>
     <col min="3" max="3" width="18.06640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -569,32 +616,32 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -602,10 +649,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -613,10 +660,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C10">
         <v>3</v>
@@ -624,65 +671,65 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C11">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A13" s="2" t="s">
-        <v>25</v>
+      <c r="A13" t="s">
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>28</v>
+      <c r="A15" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -690,10 +737,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -701,10 +748,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -712,10 +759,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -723,10 +770,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -734,10 +781,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B21" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -745,10 +792,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -756,10 +803,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -767,13 +814,115 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
         <v>45</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B26" t="s">
         <v>46</v>
       </c>
-      <c r="C24">
-        <v>1</v>
+      <c r="C26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A29" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed unnecessary inductor in BOM
</commit_message>
<xml_diff>
--- a/EFI+Ignition/PCB Files/BOM_Power_Buggy_EFI_V3.1.xlsx
+++ b/EFI+Ignition/PCB Files/BOM_Power_Buggy_EFI_V3.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53392CB3-0370-4657-979C-AC1176787E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE9D75C-4771-4306-BC93-7E11F7387122}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1073" yWindow="1073" windowWidth="18000" windowHeight="9397" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
   <si>
     <t>Description:</t>
   </si>
@@ -112,12 +112,6 @@
   </si>
   <si>
     <t>400KHz 60V 4A Switching Current Boost / Buck-Boost / Inverting DC/DC Converter</t>
-  </si>
-  <si>
-    <t>FIXED IND 33UH 4.4A 91 MOHM SMD</t>
-  </si>
-  <si>
-    <t>AMDLA1004S-330MT</t>
   </si>
   <si>
     <t>RES 150 OHM 2% 2W AXIAL</t>
@@ -563,22 +557,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="75.86328125" customWidth="1"/>
-    <col min="2" max="2" width="44.9296875" customWidth="1"/>
+    <col min="1" max="1" width="47.46484375" customWidth="1"/>
+    <col min="2" max="2" width="28.53125" customWidth="1"/>
     <col min="3" max="3" width="18.06640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -649,10 +643,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -759,10 +753,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
         <v>31</v>
-      </c>
-      <c r="B19" t="s">
-        <v>32</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -770,10 +764,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
         <v>34</v>
-      </c>
-      <c r="B20" t="s">
-        <v>33</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -781,10 +775,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" t="s">
         <v>35</v>
-      </c>
-      <c r="B21" t="s">
-        <v>36</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -803,10 +797,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -814,10 +808,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -825,10 +819,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -836,53 +830,50 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A29" s="3" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A28" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A31" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31" s="1" t="s">
+      <c r="A31" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" t="s">
         <v>53</v>
-      </c>
-      <c r="B32" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" t="s">
         <v>56</v>
-      </c>
-      <c r="B33" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.45">
@@ -915,14 +906,6 @@
       </c>
       <c r="B37" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
-        <v>65</v>
-      </c>
-      <c r="B38" t="s">
-        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>